<commit_message>
Create Test Script and Test Suites for Sprint 9
</commit_message>
<xml_diff>
--- a/TestData_Booking.xlsx
+++ b/TestData_Booking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abraham Farrendy\git\CCN-Projects-Booking-Concierge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\Cargo Community Network Pte Ltd\Booking Concierge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1026214-EE41-4B0A-8233-37CBCDE9F263}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B17D83-4620-4662-A378-81E3216D8CA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{60DB1C98-9F4E-4D24-BE07-D165FAE35515}"/>
+    <workbookView xWindow="-120" yWindow="-15720" windowWidth="29040" windowHeight="15840" xr2:uid="{60DB1C98-9F4E-4D24-BE07-D165FAE35515}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>var_AwbPrefix</t>
   </si>
@@ -114,6 +114,48 @@
   </si>
   <si>
     <t>Template004</t>
+  </si>
+  <si>
+    <t>SIN</t>
+  </si>
+  <si>
+    <t>Test Sprint 9</t>
+  </si>
+  <si>
+    <t>Sent 1st Booking</t>
+  </si>
+  <si>
+    <t>DPS</t>
+  </si>
+  <si>
+    <t>Sent 2nd Booking</t>
+  </si>
+  <si>
+    <t>vCarrierCode</t>
+  </si>
+  <si>
+    <t>vFlightNumber</t>
+  </si>
+  <si>
+    <t>vFlightDate</t>
+  </si>
+  <si>
+    <t>vBoardPoint</t>
+  </si>
+  <si>
+    <t>vOffPoint</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>var_Pieces2</t>
+  </si>
+  <si>
+    <t>var_Weight2</t>
+  </si>
+  <si>
+    <t>var_Volume2</t>
   </si>
 </sst>
 </file>
@@ -149,8 +191,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,15 +508,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39634310-F4A0-49AF-9A5C-7EF0E142ED66}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,31 +577,46 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>123</v>
       </c>
@@ -572,26 +653,156 @@
       <c r="L2" t="s">
         <v>23</v>
       </c>
-      <c r="M2">
+      <c r="R2">
         <v>111</v>
       </c>
-      <c r="N2">
+      <c r="S2">
         <v>222</v>
       </c>
-      <c r="O2">
+      <c r="T2">
         <v>121</v>
       </c>
-      <c r="P2">
+      <c r="U2">
         <v>100</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="V2" t="s">
         <v>20</v>
       </c>
-      <c r="S2" t="s">
+      <c r="X2" t="s">
         <v>16</v>
       </c>
-      <c r="T2" t="s">
+      <c r="Y2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>312</v>
+      </c>
+      <c r="B3">
+        <v>1556792</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
+      <c r="H3">
+        <v>100</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3">
+        <v>111</v>
+      </c>
+      <c r="O3" s="1">
+        <v>44012</v>
+      </c>
+      <c r="P3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3">
+        <v>112</v>
+      </c>
+      <c r="S3">
+        <v>121</v>
+      </c>
+      <c r="T3">
+        <v>122</v>
+      </c>
+      <c r="U3">
+        <v>100</v>
+      </c>
+      <c r="V3" t="s">
+        <v>20</v>
+      </c>
+      <c r="X3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>312</v>
+      </c>
+      <c r="B4">
+        <v>1556792</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>1111</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4">
+        <v>121</v>
+      </c>
+      <c r="O4" s="1">
+        <v>44012</v>
+      </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4">
+        <v>112</v>
+      </c>
+      <c r="S4">
+        <v>121</v>
+      </c>
+      <c r="T4">
+        <v>122</v>
+      </c>
+      <c r="U4">
+        <v>100</v>
+      </c>
+      <c r="V4" t="s">
+        <v>20</v>
+      </c>
+      <c r="X4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>